<commit_message>
feat: add Excel reader and enhance test logging
</commit_message>
<xml_diff>
--- a/src/test/resources/datasets.xlsx
+++ b/src/test/resources/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\selenium-project\SeleniumPomDataDriven\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F48F69-616A-49EE-B607-E2E766074310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E97FA9-BC34-4657-909C-B6ED80374582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Value1</t>
   </si>
@@ -53,16 +53,10 @@
     <t>hectometers [hm]</t>
   </si>
   <si>
-    <t>micrometers [µm]</t>
-  </si>
-  <si>
     <t>nanometers [nm]</t>
   </si>
   <si>
     <t>millimeters [mm]</t>
-  </si>
-  <si>
-    <t>0.123456789</t>
   </si>
   <si>
     <t>Convert Time</t>
@@ -108,9 +102,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -182,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,43 +188,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,7 +504,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,12 +516,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -549,13 +538,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>12.5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>12500</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -563,44 +552,38 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
+      <c r="A4" s="7">
+        <v>1.234</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9">
-        <v>12345678.9</v>
+      <c r="C4" s="14">
+        <v>0.1234</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1000000</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -628,80 +611,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>325.75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4">
+        <v>325750</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="14" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>325.75</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5">
-        <v>325750</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0.51249999999999996</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="5">
+        <v>512.5</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>0.51249999999999996</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6">
-        <v>512.5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -729,80 +706,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1.57</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6">
+        <v>94.2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7">
-        <v>94.2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="5">
-        <v>30</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>